<commit_message>
analytical solution matrix game 2x2
</commit_message>
<xml_diff>
--- a/core/src/main/resources/data.xlsx
+++ b/core/src/main/resources/data.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Чистые стратегии" sheetId="1" r:id="rId1"/>
     <sheet name="Смешанные стратегии" sheetId="2" r:id="rId2"/>
     <sheet name="Редукция" sheetId="3" r:id="rId3"/>
-    <sheet name="Лист1" sheetId="4" r:id="rId4"/>
+    <sheet name="2X2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -361,54 +361,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>-8</v>
+      </c>
+      <c r="C1">
+        <v>-7</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-4</v>
+      </c>
+      <c r="B2">
+        <v>-5</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>-5</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>-5</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>-4</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>-5</v>
+      </c>
+      <c r="C5">
+        <v>-4</v>
+      </c>
+      <c r="D5">
+        <v>-3</v>
+      </c>
+      <c r="E5">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
@@ -421,53 +464,51 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>8</v>
+        <v>-4</v>
       </c>
       <c r="B1">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C1">
         <v>-7</v>
       </c>
+      <c r="D1">
+        <v>-5</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>-5</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>-6</v>
+      </c>
+      <c r="D2">
+        <v>-7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="B3">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="C3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-4</v>
-      </c>
-      <c r="B4">
-        <v>-2</v>
-      </c>
-      <c r="C4">
-        <v>-5</v>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -475,16 +516,13 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.36364000000000002</v>
       </c>
       <c r="D5">
-        <v>0.375</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
+        <v>0.63636000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -492,13 +530,16 @@
         <v>1</v>
       </c>
       <c r="B6">
+        <v>0.54544999999999999</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>0.8125</v>
-      </c>
       <c r="D6">
-        <v>0.1875</v>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.45455000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -508,148 +549,127 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-73</v>
+        <v>-58</v>
       </c>
       <c r="B1">
-        <v>-54</v>
+        <v>-17</v>
       </c>
       <c r="C1">
-        <v>-56</v>
+        <v>-44</v>
       </c>
       <c r="D1">
-        <v>-35</v>
+        <v>-31</v>
       </c>
       <c r="E1">
-        <v>-64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F1">
+        <v>16</v>
+      </c>
+      <c r="G1">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-37</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>-70</v>
+        <v>-12</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>-42</v>
       </c>
       <c r="D2">
-        <v>-22</v>
+        <v>-53</v>
       </c>
       <c r="E2">
-        <v>-31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-32</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-37</v>
+        <v>36</v>
       </c>
       <c r="B3">
-        <v>-44</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>44</v>
+        <v>-42</v>
       </c>
       <c r="D3">
-        <v>-73</v>
+        <v>38</v>
       </c>
       <c r="E3">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>37</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-66</v>
+        <v>-49</v>
       </c>
       <c r="B4">
         <v>-72</v>
       </c>
       <c r="C4">
-        <v>-63</v>
+        <v>27</v>
       </c>
       <c r="D4">
+        <v>-13</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>-14</v>
+      </c>
+      <c r="C5">
+        <v>-48</v>
+      </c>
+      <c r="D5">
+        <v>-10</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+      <c r="F5">
         <v>-25</v>
       </c>
-      <c r="E4">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>-37</v>
-      </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-      <c r="C5">
-        <v>22</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>-58</v>
-      </c>
-      <c r="B6">
-        <v>29</v>
-      </c>
-      <c r="C6">
-        <v>-56</v>
-      </c>
-      <c r="D6">
-        <v>-29</v>
-      </c>
-      <c r="E6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>-6</v>
-      </c>
-      <c r="B7">
-        <v>-65</v>
-      </c>
-      <c r="C7">
-        <v>-50</v>
-      </c>
-      <c r="D7">
-        <v>-62</v>
-      </c>
-      <c r="E7">
-        <v>-31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>-3</v>
-      </c>
-      <c r="B8">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>41</v>
-      </c>
-      <c r="D8">
-        <v>-27</v>
-      </c>
-      <c r="E8">
-        <v>16</v>
+      <c r="G5">
+        <v>-18</v>
       </c>
     </row>
   </sheetData>
@@ -659,127 +679,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-58</v>
+        <v>17</v>
       </c>
       <c r="B1">
-        <v>-17</v>
-      </c>
-      <c r="C1">
-        <v>-44</v>
-      </c>
-      <c r="D1">
-        <v>-31</v>
-      </c>
-      <c r="E1">
-        <v>17</v>
-      </c>
-      <c r="F1">
-        <v>16</v>
-      </c>
-      <c r="G1">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>-12</v>
-      </c>
-      <c r="C2">
-        <v>-42</v>
-      </c>
-      <c r="D2">
-        <v>-53</v>
-      </c>
-      <c r="E2">
-        <v>-32</v>
-      </c>
-      <c r="F2">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>36</v>
-      </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>-42</v>
-      </c>
-      <c r="D3">
-        <v>38</v>
-      </c>
-      <c r="E3">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>37</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-49</v>
-      </c>
-      <c r="B4">
-        <v>-72</v>
-      </c>
-      <c r="C4">
-        <v>27</v>
-      </c>
-      <c r="D4">
-        <v>-13</v>
-      </c>
-      <c r="E4">
-        <v>32</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>-14</v>
-      </c>
-      <c r="C5">
-        <v>-48</v>
-      </c>
-      <c r="D5">
-        <v>-10</v>
-      </c>
-      <c r="E5">
-        <v>17</v>
-      </c>
-      <c r="F5">
-        <v>-25</v>
-      </c>
-      <c r="G5">
-        <v>-18</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>